<commit_message>
Artikel: Berkas Pajak: Restructure
</commit_message>
<xml_diff>
--- a/assets/posts/pajak/2018/03/Teliti-2018-SSE.xlsx
+++ b/assets/posts/pajak/2018/03/Teliti-2018-SSE.xlsx
@@ -344,7 +344,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -364,10 +368,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,7 +388,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,7 +404,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,7 +412,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,7 +436,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,7 +444,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,7 +460,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -555,40 +555,40 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,6 +974,7 @@
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="15"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B40" s="13"/>

</xml_diff>

<commit_message>
Artikel: Berkas Pajak: Change CoA Name
</commit_message>
<xml_diff>
--- a/assets/posts/pajak/2018/03/Teliti-2018-SSE.xlsx
+++ b/assets/posts/pajak/2018/03/Teliti-2018-SSE.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Bambang Rudolfo</t>
   </si>
   <si>
-    <t xml:space="preserve">09.254.294.3-407.000</t>
+    <t xml:space="preserve">09.254.294.3-405.000</t>
   </si>
   <si>
     <t xml:space="preserve">PPh 4(2)</t>
@@ -555,8 +555,8 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>

</xml_diff>